<commit_message>
Fixed error in processing code - rerunning relevant models. 6 NA's due to single letter mistake in animal conversion
</commit_message>
<xml_diff>
--- a/Data processing/LO_compcase_es.xlsx
+++ b/Data processing/LO_compcase_es.xlsx
@@ -49585,7 +49585,7 @@
         <v>24</v>
       </c>
       <c r="AA502">
-        <v>-0.5860025431086175</v>
+        <v>-0.5860025431086177</v>
       </c>
       <c r="AB502">
         <v>0.1816590272472625</v>
@@ -51349,7 +51349,7 @@
         <v>19</v>
       </c>
       <c r="AA520">
-        <v>0.3206262281711347</v>
+        <v>0.3206262281711348</v>
       </c>
       <c r="AB520">
         <v>0.1814194577352472</v>

</xml_diff>